<commit_message>
Add excel sheet, remove card number addition,
</commit_message>
<xml_diff>
--- a/card_data.xlsx
+++ b/card_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,6 +421,9 @@
       <c r="F1" t="str">
         <v>Timestamp</v>
       </c>
+      <c r="G1" t="str">
+        <v>Phone</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -482,9 +485,52 @@
         <v>11/2/2025, 3:39:21 PM</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>JOHN DOE</v>
+      </c>
+      <c r="B5" t="str">
+        <v>ahmed@gmail.com</v>
+      </c>
+      <c r="C5" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D5" t="str">
+        <v>12/∞</v>
+      </c>
+      <c r="E5" t="str">
+        <v>985</v>
+      </c>
+      <c r="F5" t="str">
+        <v>11/13/2025, 12:03:28 PM</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>JOHN DOE</v>
+      </c>
+      <c r="B6" t="str">
+        <v>johny@gmail.com</v>
+      </c>
+      <c r="C6" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D6" t="str">
+        <v>12/∞</v>
+      </c>
+      <c r="E6" t="str">
+        <v>985</v>
+      </c>
+      <c r="F6" t="str">
+        <v>11/13/2025, 12:16:14 PM</v>
+      </c>
+      <c r="G6" t="str">
+        <v>+963993625082</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove the expiry data and card number
</commit_message>
<xml_diff>
--- a/card_data.xlsx
+++ b/card_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -528,9 +528,32 @@
         <v>+963993625082</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>JOHN DOE</v>
+      </c>
+      <c r="B7" t="str">
+        <v>nicolas@gmail.com</v>
+      </c>
+      <c r="C7" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D7" t="str">
+        <v>12-∞</v>
+      </c>
+      <c r="E7" t="str">
+        <v>985</v>
+      </c>
+      <c r="F7" t="str">
+        <v>11/17/2025, 10:41:35 AM</v>
+      </c>
+      <c r="G7" t="str">
+        <v>963993625082</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes to add three versions of cards
</commit_message>
<xml_diff>
--- a/card_data.xlsx
+++ b/card_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -551,9 +551,78 @@
         <v>963993625082</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>WAssem</v>
+      </c>
+      <c r="B8" t="str">
+        <v>was@jjj.com</v>
+      </c>
+      <c r="C8" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D8" t="str">
+        <v>12-∞</v>
+      </c>
+      <c r="E8" t="str">
+        <v>985</v>
+      </c>
+      <c r="F8" t="str">
+        <v>11/18/2025, 4:23:28 PM</v>
+      </c>
+      <c r="G8" t="str">
+        <v>+963879394</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Ahmad Bassam Abboud</v>
+      </c>
+      <c r="B9" t="str">
+        <v>student@university.edu</v>
+      </c>
+      <c r="C9" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D9" t="str">
+        <v>12-∞</v>
+      </c>
+      <c r="E9" t="str">
+        <v>985</v>
+      </c>
+      <c r="F9" t="str">
+        <v>11/18/2025, 4:23:58 PM</v>
+      </c>
+      <c r="G9" t="str">
+        <v>+963879394</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>test</v>
+      </c>
+      <c r="B10" t="str">
+        <v>test@mail.com</v>
+      </c>
+      <c r="C10" t="str">
+        <v>7007********5055</v>
+      </c>
+      <c r="D10" t="str">
+        <v>12-∞</v>
+      </c>
+      <c r="E10" t="str">
+        <v>985</v>
+      </c>
+      <c r="F10" t="str">
+        <v>11/18/2025, 4:24:11 PM</v>
+      </c>
+      <c r="G10" t="str">
+        <v>1723871893</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>